<commit_message>
Fix screenshot for all report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCRM/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdataCRM/ClientsDataExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT_FRAMEWORK\AutomationFrameworkSelenium\src\test\resources\testdataCRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9FDB16-4B1B-4CE5-BB6F-D0A79BF36E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999B4FAD-B525-4015-BA28-ECC0470155F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -100,15 +100,6 @@
     <t>VIP</t>
   </si>
   <si>
-    <t>admin@demo.com</t>
-  </si>
-  <si>
-    <t>dw5AQDhu9+WsEsWisMJISA==</t>
-  </si>
-  <si>
-    <t>client@demo.com</t>
-  </si>
-  <si>
     <t>Gold</t>
   </si>
   <si>
@@ -158,6 +149,15 @@
   </si>
   <si>
     <t>SA</t>
+  </si>
+  <si>
+    <t>admin@example.com</t>
+  </si>
+  <si>
+    <t>client@example.com</t>
+  </si>
+  <si>
+    <t>T+wyT5u9cOelDJbBWNgxLw==</t>
   </si>
 </sst>
 </file>
@@ -329,13 +329,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -355,9 +355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -395,7 +395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -501,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -653,15 +653,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.296875" style="10" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.19921875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.09765625" style="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.19921875" style="10" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.796875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
@@ -693,13 +693,13 @@
       <c r="A2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="14"/>
+      <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="13"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -709,11 +709,11 @@
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>25</v>
+      <c r="B3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E2E380-41FF-438A-822D-1CBE2A443631}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.19921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -796,7 +796,7 @@
         <v>15</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>13</v>
@@ -807,25 +807,25 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G2" s="3">
         <v>1001</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3">
         <v>123456</v>
@@ -840,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -848,25 +848,25 @@
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>1002</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I3" s="3">
         <v>123456</v>
@@ -878,10 +878,10 @@
         <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -889,25 +889,25 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="G4" s="3">
         <v>1003</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I4" s="3">
         <v>123456</v>
@@ -922,7 +922,7 @@
         <v>23</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update version 2.4.8 upgrade Selenium 4.27.0
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCRM/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdataCRM/ClientsDataExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT_FRAMEWORK\AutomationFrameworkSelenium\src\test\resources\testdataCRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999B4FAD-B525-4015-BA28-ECC0470155F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9EEB5B-8318-401E-AB57-AE20F46AC1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>VAT</t>
   </si>
@@ -103,15 +103,6 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Mark Thomas</t>
-  </si>
-  <si>
-    <t>Richard Gray</t>
-  </si>
-  <si>
-    <t>Sara Ann</t>
-  </si>
-  <si>
     <t>APPLICATION</t>
   </si>
   <si>
@@ -124,12 +115,6 @@
     <t>eCommerce</t>
   </si>
   <si>
-    <t>Anh Tester Client 0108A1</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 0108A2</t>
-  </si>
-  <si>
     <t>Anh Tester Client 0108A3</t>
   </si>
   <si>
@@ -158,6 +143,30 @@
   </si>
   <si>
     <t>T+wyT5u9cOelDJbBWNgxLw==</t>
+  </si>
+  <si>
+    <t>Admin Example</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 1812A1</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 1812A2</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>Can Tho</t>
+  </si>
+  <si>
+    <t>Tra Vinh</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>TV</t>
   </si>
 </sst>
 </file>
@@ -653,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -694,10 +703,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="11"/>
@@ -710,10 +719,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -735,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E2E380-41FF-438A-822D-1CBE2A443631}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.19921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -796,7 +805,7 @@
         <v>15</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>13</v>
@@ -807,25 +816,25 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G2" s="3">
         <v>1001</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I2" s="3">
         <v>123456</v>
@@ -840,7 +849,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -848,25 +857,25 @@
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G3" s="3">
         <v>1002</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I3" s="3">
         <v>123456</v>
@@ -881,7 +890,7 @@
         <v>24</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -889,25 +898,25 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G4" s="3">
         <v>1003</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I4" s="3">
         <v>123456</v>
@@ -922,7 +931,7 @@
         <v>23</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>